<commit_message>
1st week last update
</commit_message>
<xml_diff>
--- a/document/調査メモ.xlsx
+++ b/document/調査メモ.xlsx
@@ -277,10 +277,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>HSQLDBの使い方</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>http://www.wakhok.ac.jp/~tomoharu/jsf2004/hsqldb/</t>
-  </si>
-  <si>
-    <t>HSQLDBの使い方</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -288,7 +289,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +304,14 @@
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -322,17 +331,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -694,15 +711,18 @@
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add work of 0823
</commit_message>
<xml_diff>
--- a/document/調査メモ.xlsx
+++ b/document/調査メモ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>https://flywaydb.org/</t>
   </si>
@@ -282,6 +282,105 @@
   </si>
   <si>
     <t>http://www.wakhok.ac.jp/~tomoharu/jsf2004/hsqldb/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Spring Bootで静的コンテンツを配置</t>
+    <rPh sb="12" eb="14">
+      <t>セイテキ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ハイチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/src/main/resources/static配下に配置</t>
+    <rPh sb="26" eb="28">
+      <t>ハイカ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ハイチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>リンクは/src/main/resources/static以下のパスを記述</t>
+    <rPh sb="30" eb="32">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>キジュツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://qiita.com/hiroshi_maz/items/0a7eec94e9a4ec1413f1</t>
+  </si>
+  <si>
+    <t>→application.propertiesに以下の記述があると、テンプレートや静的ファイルの更新時にアプリケーションの再起動が不要</t>
+    <rPh sb="24" eb="26">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>キジュツ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>セイテキ</t>
+    </rPh>
+    <rPh sb="48" eb="51">
+      <t>コウシンジ</t>
+    </rPh>
+    <rPh sb="61" eb="64">
+      <t>サイキドウ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>フヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>spring.thymeleaf.cache=false</t>
+  </si>
+  <si>
+    <t>spring.jpa.hibernate.ddl-auto=update</t>
+  </si>
+  <si>
+    <t>JPAで接続してデータがきちんと永続化されるようにapplication.propertiesに以下の行を追加する</t>
+    <rPh sb="4" eb="6">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>エイゾクカ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>ギョウ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※この行がないとJPA経由で接続したとき、アプリが終了するとデータが削除される</t>
+    <rPh sb="3" eb="4">
+      <t>ギョウ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ケイユ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>サクジョ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -642,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -653,7 +752,7 @@
     <col min="2" max="2" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -664,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -672,12 +771,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -688,7 +787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -696,32 +795,75 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C21" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
+    <hyperlink ref="B21" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>